<commit_message>
updating, mostly tracker files no changes to code that I remember
</commit_message>
<xml_diff>
--- a/PILE flags_QAQC 2024-03-07 .xlsx
+++ b/PILE flags_QAQC 2024-03-07 .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/edeegan_nps_gov/Documents/FFIqaqc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="11_D11E2FCFECCCE5EF932B40A8CDA073F1BF302E43" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DA92860-2209-4C3E-9625-ED4EFFE7AEF5}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="11_D11E2FCFECCCE5EF932B40A8CDA073F1BF302E43" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD0BEBE3-223E-4F47-B224-8FDEAC81CCB8}"/>
   <bookViews>
-    <workbookView xWindow="22710" yWindow="-15870" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22710" yWindow="-15870" windowWidth="25440" windowHeight="15390" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PILE-01" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,12 @@
     <sheet name="Comments" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="107">
   <si>
     <t>Issue</t>
   </si>
@@ -273,6 +274,81 @@
   </si>
   <si>
     <t>this is for seedlings which isn't specified in flag unfortunately</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>ESD 3/18/24</t>
+  </si>
+  <si>
+    <t>unclear</t>
+  </si>
+  <si>
+    <t>no crown class recorded - nothing to do</t>
+  </si>
+  <si>
+    <t>no crown class recorded because it was on pole data sheet even with dbh of 16, nothing to do</t>
+  </si>
+  <si>
+    <t>no crown class recorded</t>
+  </si>
+  <si>
+    <t>change to recent snag or delete</t>
+  </si>
+  <si>
+    <t>data sheet says recent dead with no crown class</t>
+  </si>
+  <si>
+    <t>delete crown class</t>
+  </si>
+  <si>
+    <t>just dead no crown class recorded</t>
+  </si>
+  <si>
+    <t>note in QAQC</t>
+  </si>
+  <si>
+    <t>no crown class recorded, tree is alive</t>
+  </si>
+  <si>
+    <t>crown  class was valid before 2002 (?)</t>
+  </si>
+  <si>
+    <t>confirmed with data sheet</t>
+  </si>
+  <si>
+    <t>unclear why this was flagged</t>
+  </si>
+  <si>
+    <t>nothing on seedling sheet says shrub, species code is ARPU for both which on species list is a shrub, is this allowed?</t>
+  </si>
+  <si>
+    <t>ask Windy</t>
+  </si>
+  <si>
+    <t>0 was a placeholder for pole trees with no tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">two trees tagged for each of these numbers, an overstory and a pole -not sure what to do but it’s a problem </t>
+  </si>
+  <si>
+    <t>change 2005 to resting dbh from 2001</t>
+  </si>
+  <si>
+    <t>has to be a different tree dbh goes from 39 to 16.8, but the same species, not sure what to do</t>
+  </si>
+  <si>
+    <t>change 2015 to resting dbh from 2014</t>
+  </si>
+  <si>
+    <t>placeholder, tagged with letters</t>
+  </si>
+  <si>
+    <t>change 2005 to 2001 resting dbh</t>
+  </si>
+  <si>
+    <t>change 2005 to resting dbh from 2002</t>
   </si>
 </sst>
 </file>
@@ -614,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -643,6 +719,15 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
       </c>
       <c r="E2" t="s">
         <v>81</v>
@@ -741,7 +826,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E5"/>
+      <selection activeCell="B17" sqref="B17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -770,11 +855,32 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -994,24 +1100,69 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1026,7 +1177,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E5"/>
+      <selection activeCell="B9" sqref="B9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1055,11 +1206,32 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -1146,6 +1318,18 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1160,7 +1344,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E5"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1189,11 +1373,32 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -1335,15 +1540,48 @@
       <c r="A12" t="s">
         <v>20</v>
       </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1358,7 +1596,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1387,70 +1625,217 @@
       <c r="A2" t="s">
         <v>22</v>
       </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>29</v>
       </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
+      <c r="B14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1464,7 +1849,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1493,6 +1878,18 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -1634,20 +2031,62 @@
       <c r="A11" t="s">
         <v>37</v>
       </c>
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>38</v>
       </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1661,8 +2100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1691,6 +2130,18 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -1832,11 +2283,32 @@
       <c r="A11" t="s">
         <v>41</v>
       </c>
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>31</v>
       </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1846,17 +2318,41 @@
         <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>42</v>
       </c>
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PILE flags modified and i&M script add to file - not currently using but could be used for metadata in the future
</commit_message>
<xml_diff>
--- a/PILE flags_QAQC 2024-03-07 .xlsx
+++ b/PILE flags_QAQC 2024-03-07 .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/edeegan_nps_gov/Documents/FFIqaqc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="11_D11E2FCFECCCE5EF932B40A8CDA073F1BF302E43" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD0BEBE3-223E-4F47-B224-8FDEAC81CCB8}"/>
+  <xr:revisionPtr revIDLastSave="205" documentId="11_D11E2FCFECCCE5EF932B40A8CDA073F1BF302E43" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B6BCD20-BD08-46BA-8C5C-4566869F0581}"/>
   <bookViews>
-    <workbookView xWindow="22710" yWindow="-15870" windowWidth="25440" windowHeight="15390" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PILE-01" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,11 @@
     <sheet name="Comments" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="108">
   <si>
     <t>Issue</t>
   </si>
@@ -349,6 +348,9 @@
   </si>
   <si>
     <t>change 2005 to resting dbh from 2002</t>
+  </si>
+  <si>
+    <t>this is for seedlings which isn't specified in flag unfortunately, Note in datasheet says all quercus seedlings recorded in brush belts, all other species in Q1/Q2 (but what size subplot? The subfraction recorded seems to suggest they sampled in two 5x10m microplots)</t>
   </si>
 </sst>
 </file>
@@ -690,16 +692,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="114" customWidth="1"/>
+    <col min="1" max="1" width="135.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -716,7 +722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -730,10 +736,10 @@
         <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -750,7 +756,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -767,7 +773,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -784,7 +790,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -801,7 +807,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -825,16 +831,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:E17"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="125.36328125" customWidth="1"/>
+    <col min="1" max="1" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -851,7 +861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -865,7 +875,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -882,7 +892,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -899,7 +909,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -916,7 +926,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -933,7 +943,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -950,7 +960,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -967,7 +977,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -984,7 +994,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1001,7 +1011,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1018,7 +1028,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1035,7 +1045,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1052,7 +1062,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1069,7 +1079,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1086,7 +1096,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1100,7 +1110,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1117,7 +1127,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1134,7 +1144,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1148,7 +1158,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1177,15 +1187,19 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:E9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="114" customWidth="1"/>
+    <col min="1" max="1" width="174.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1202,7 +1216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1216,7 +1230,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1233,7 +1247,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1250,7 +1264,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1267,7 +1281,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1284,7 +1298,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1301,7 +1315,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1315,7 +1329,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1344,15 +1358,19 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="122.08984375" customWidth="1"/>
+    <col min="1" max="1" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="85.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1369,7 +1387,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1383,7 +1401,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1400,7 +1418,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1417,7 +1435,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1434,7 +1452,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1451,7 +1469,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1468,7 +1486,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1485,7 +1503,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1502,7 +1520,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1519,7 +1537,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1536,7 +1554,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1553,7 +1571,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1567,7 +1585,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1595,16 +1613,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="121.36328125" customWidth="1"/>
+    <col min="1" max="1" width="171.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="105.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1621,7 +1643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1638,7 +1660,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1652,7 +1674,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1669,7 +1691,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1683,7 +1705,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1700,7 +1722,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1714,7 +1736,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1731,7 +1753,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1745,7 +1767,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1762,7 +1784,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1776,7 +1798,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1790,7 +1812,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1807,7 +1829,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1821,7 +1843,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1849,15 +1871,19 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="145.26953125" customWidth="1"/>
+    <col min="1" max="1" width="173.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1874,7 +1900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1891,7 +1917,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1908,7 +1934,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1925,7 +1951,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1942,7 +1968,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1959,7 +1985,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1976,7 +2002,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1993,7 +2019,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2010,7 +2036,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2027,7 +2053,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -2044,7 +2070,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2058,7 +2084,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -2075,7 +2101,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -2100,16 +2126,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="109.26953125" customWidth="1"/>
+    <col min="1" max="1" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2126,7 +2156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2143,7 +2173,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2160,7 +2190,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -2177,7 +2207,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -2194,7 +2224,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -2211,7 +2241,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -2228,7 +2258,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -2245,7 +2275,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -2262,7 +2292,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -2279,7 +2309,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -2296,7 +2326,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -2310,7 +2340,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2324,7 +2354,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -2341,7 +2371,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2366,11 +2396,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2387,162 +2422,162 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>74</v>
       </c>

</xml_diff>